<commit_message>
Started writing the simulation writeup report
</commit_message>
<xml_diff>
--- a/FEMM Simulations/Data/ProjectileLength 2019_10_08 15_01/7mmCoil_192T_156A_swProjectileLength.xlsx
+++ b/FEMM Simulations/Data/ProjectileLength 2019_10_08 15_01/7mmCoil_192T_156A_swProjectileLength.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekultho\Documents\Personal\CG 490\FEMM Simulations\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekultho\Documents\Personal\CG 490\FEMM Simulations\Data\ProjectileLength 2019_10_08 15_01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F7371F-DA85-4DD6-9868-7D1C8A51DCFF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7501FF-2FE8-4220-876F-549404CC49C5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1008" yWindow="948" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -7761,8 +7761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G22" workbookViewId="0">
-      <selection activeCell="S64" sqref="S64"/>
+    <sheetView tabSelected="1" topLeftCell="G15" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9671,11 +9671,11 @@
         <v>0.11376623178726381</v>
       </c>
       <c r="H40">
-        <f t="array" ref="H40">SUM(ABS(H$2:H2))*0.1</f>
+        <f>SUM(ABS(H$2:H2))*0.1</f>
         <v>0.1293916697659114</v>
       </c>
       <c r="I40">
-        <f t="array" ref="I40">SUM(ABS(I$2:I2))*0.1</f>
+        <f>SUM(ABS(I$2:I2))*0.1</f>
         <v>0.13525572134793531</v>
       </c>
       <c r="J40">
@@ -9683,7 +9683,7 @@
         <v>0.14547368358819121</v>
       </c>
       <c r="K40">
-        <f t="array" ref="K40">SUM(ABS(K$2:K2))*0.1</f>
+        <f>SUM(ABS(K$2:K2))*0.1</f>
         <v>0.1584496525416175</v>
       </c>
       <c r="L40">
@@ -9849,9 +9849,9 @@
         <f t="array" ref="I43">SUM(ABS(I$2:I5))*0.1</f>
         <v>3.6142144852291511</v>
       </c>
-      <c r="J43">
-        <f t="array" ref="J43">SUM(ABS(J$2:J5))*0.1</f>
-        <v>3.6741262858442525</v>
+      <c r="J43" t="e">
+        <f>SUM(ABS(J$2:J5))*0.1</f>
+        <v>#VALUE!</v>
       </c>
       <c r="K43">
         <f t="array" ref="K43">SUM(ABS(K$2:K5))*0.1</f>

</xml_diff>